<commit_message>
update plan 20201119 & update result 20201118
</commit_message>
<xml_diff>
--- a/20201118.xlsx
+++ b/20201118.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swan3\Desktop\plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC99058-83F8-4666-9167-3946665CCD7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567FC102-E6AE-4482-875A-8B3A3454F207}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23844" yWindow="1152" windowWidth="21600" windowHeight="11328" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-120" windowWidth="23256" windowHeight="12576" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -32,18 +32,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>일</t>
   </si>
   <si>
-    <t>수행</t>
-  </si>
-  <si>
     <t>휴식</t>
-  </si>
-  <si>
-    <t>내용</t>
   </si>
   <si>
     <t>시간</t>
@@ -113,9 +107,6 @@
     <t>13:00 ~ 15:00</t>
   </si>
   <si>
-    <t>9:00 ~ 11:20</t>
-  </si>
-  <si>
     <t>15:00 ~ 15:10</t>
   </si>
   <si>
@@ -128,16 +119,9 @@
     <t>17:20 ~ 18:00</t>
   </si>
   <si>
-    <t xml:space="preserve">8:10 ~ 8:55  </t>
-  </si>
-  <si>
     <t>18:00 ~ 19:10</t>
   </si>
   <si>
-    <t>출근시간(45분) / 전자기학</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
     <t>비고</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
@@ -171,10 +155,6 @@
   </si>
   <si>
     <t>21:50 ~ 22:30</t>
-    <phoneticPr fontId="21" type="noConversion"/>
-  </si>
-  <si>
-    <t>퇴근시간(45분)</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
   <si>
@@ -220,6 +200,59 @@
   </si>
   <si>
     <t>네트워크 로그 분리 &amp; 충전중 cp stat 9번 주기전송</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>할 일</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 오마카세 예약</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 2채널
+ - 온도센서관련 이슈 테스트
+  -&gt; 불량 4EA는 불량 아님?
+2. 모빌리티
+ - 미팅 전 체크
+  -&gt; 위지온 서버와 연결 확인 및 데이터 검증(진행중)
+3. BMK 24v 
+ - 진행안함
+4. F7
+ - 로그 분리(진행중)
+  -&gt;네트워크와 시스템로그를 분리
+ - CP stat9번 전송
+  -&gt;완료화면에서 충전커넥터가 빠지지 않을 경우 cp stat을 9로 하여 주기적으로 34번전문을 전송  
+     한다.</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>늦잠</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>요즘은 회사에서 작성한다.</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>사유</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>출근시간(45분) / 전자기학</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>퇴근시간(45분) / 전자기학</t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">8:10 ~ 8:55  </t>
+    <phoneticPr fontId="21" type="noConversion"/>
+  </si>
+  <si>
+    <t>8:55 ~ 11:20</t>
     <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
@@ -393,7 +426,7 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -608,6 +641,24 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -913,7 +964,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -923,77 +974,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="1" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1007,23 +1046,38 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="176" fontId="1" fillId="38" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="38" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1557,389 +1611,402 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B2:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="16.5" customWidth="1"/>
-    <col min="3" max="3" width="48.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.125" customWidth="1"/>
-    <col min="6" max="6" width="85.75" customWidth="1"/>
-    <col min="7" max="7" width="18.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.875" customWidth="1"/>
-    <col min="9" max="9" width="39.75" customWidth="1"/>
-    <col min="11" max="11" width="9.875" customWidth="1"/>
+    <col min="3" max="3" width="48.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.09765625" customWidth="1"/>
+    <col min="5" max="5" width="85.69921875" customWidth="1"/>
+    <col min="6" max="6" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.8984375" customWidth="1"/>
+    <col min="9" max="9" width="39.69921875" customWidth="1"/>
+    <col min="11" max="11" width="9.8984375" customWidth="1"/>
     <col min="12" max="12" width="78" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="11"/>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="23"/>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>10</v>
       </c>
-      <c r="L2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="27"/>
+    </row>
+    <row r="3" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>50</v>
+      </c>
       <c r="G3" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="23"/>
+        <v>43</v>
+      </c>
+      <c r="H3" s="11"/>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="J3">
         <v>36</v>
       </c>
       <c r="K3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="28"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B4" s="26"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="32"/>
       <c r="G4" s="35"/>
-      <c r="H4" s="23"/>
+      <c r="H4" s="11"/>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J4">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="28"/>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B5" s="26"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="32"/>
       <c r="G5" s="35"/>
-      <c r="H5" s="23"/>
+      <c r="H5" s="11"/>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J5">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="28"/>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B6" s="26"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="32"/>
       <c r="G6" s="35"/>
-      <c r="H6" s="23"/>
+      <c r="H6" s="11"/>
       <c r="I6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J6">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="28"/>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B7" s="26"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="32"/>
       <c r="G7" s="35"/>
-      <c r="H7" s="23"/>
+      <c r="H7" s="11"/>
       <c r="I7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J7">
         <f>SUM(J3:J6)</f>
         <v>206</v>
       </c>
       <c r="L7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="28"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B8" s="26"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="32"/>
       <c r="G8" s="35"/>
-      <c r="H8" s="23"/>
+      <c r="H8" s="11"/>
       <c r="I8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J8">
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="28"/>
+    <row r="9" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="32"/>
       <c r="G9" s="35"/>
-      <c r="H9" s="23"/>
+      <c r="H9" s="11"/>
       <c r="I9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J9">
         <v>309</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="28"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B10" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="20"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="32"/>
       <c r="G10" s="35"/>
-      <c r="H10" s="23"/>
-    </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.4">
       <c r="B11" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="20"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="11"/>
+    </row>
+    <row r="13" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="20"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.4">
+      <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="20"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="11"/>
+    </row>
+    <row r="16" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="20"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B18" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="11"/>
+    </row>
+    <row r="19" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="20"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B20" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="20"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="11"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B22" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="20"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="11"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B23" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="11"/>
+    </row>
+    <row r="24" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="24"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="23"/>
-    </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="23"/>
-    </row>
-    <row r="13" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="23"/>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B14" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="24"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="23"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B15" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="24"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="23"/>
-    </row>
-    <row r="16" spans="2:13" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="23"/>
-    </row>
-    <row r="17" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" s="24"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="23"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="23"/>
-    </row>
-    <row r="19" spans="2:8" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="23"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="10" t="s">
+      <c r="C24" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="24"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="23"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="23"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="23"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="23"/>
-    </row>
-    <row r="24" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="28"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="33"/>
       <c r="G24" s="36"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="G3:G24"/>
-    <mergeCell ref="F3:F24"/>
+  <mergeCells count="8">
+    <mergeCell ref="G3:G14"/>
+    <mergeCell ref="G15:G24"/>
+    <mergeCell ref="E3:E24"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C3:C8"/>
     <mergeCell ref="D3:D8"/>
-    <mergeCell ref="E3:E8"/>
+    <mergeCell ref="F3:F14"/>
+    <mergeCell ref="F15:F24"/>
   </mergeCells>
   <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
@@ -1954,7 +2021,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>
@@ -1969,7 +2036,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <sheetData/>
   <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.69986110925674438" right="0.69986110925674438" top="0.75" bottom="0.75" header="0.30000001192092896" footer="0.30000001192092896"/>

</xml_diff>